<commit_message>
Added Plant health index with comparison plot
additionally a column with total hi values was created
</commit_message>
<xml_diff>
--- a/02_output/09_plant_health/combined_plant_data_rp.xlsx
+++ b/02_output/09_plant_health/combined_plant_data_rp.xlsx
@@ -2325,7 +2325,9 @@
       <c r="E70" t="s">
         <v>54</v>
       </c>
-      <c r="F70"/>
+      <c r="F70" t="n">
+        <v>1</v>
+      </c>
       <c r="G70" t="s">
         <v>17</v>
       </c>

</xml_diff>